<commit_message>
Nagyobb import, összevont órák(még csak 2 osztály), SolverConfig
</commit_message>
<xml_diff>
--- a/import.xlsx
+++ b/import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berta\IdeaProjects\SchoolTimeTableM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A5F7C2-81DE-43A3-9300-4E2219048921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F2CA62-F1B5-4683-8151-7F0BADA55952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="36">
   <si>
     <t>Math</t>
   </si>
@@ -135,6 +135,18 @@
   </si>
   <si>
     <t>Tanár2(bontott óra esetén)</t>
+  </si>
+  <si>
+    <t>Osztály2(összevont óra esetén)</t>
+  </si>
+  <si>
+    <t>Tömbösítés Azonosító</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -208,12 +220,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -749,67 +762,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="7" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="5" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5" t="s">
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5" t="s">
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AM1" s="5"/>
-      <c r="AN1" s="5"/>
-      <c r="AO1" s="5"/>
-      <c r="AP1" s="5"/>
-      <c r="AQ1" s="5"/>
-      <c r="AR1" s="5"/>
-      <c r="AS1" s="5"/>
-      <c r="AT1" s="5"/>
+      <c r="AM1" s="6"/>
+      <c r="AN1" s="6"/>
+      <c r="AO1" s="6"/>
+      <c r="AP1" s="6"/>
+      <c r="AQ1" s="6"/>
+      <c r="AR1" s="6"/>
+      <c r="AS1" s="6"/>
+      <c r="AT1" s="6"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="2">
         <v>1</v>
       </c>
@@ -1702,15 +1715,15 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Munka2"/>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1723,9 +1736,14 @@
       <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1738,8 +1756,11 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1752,8 +1773,11 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1763,8 +1787,11 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1775,7 +1802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1786,7 +1813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1797,7 +1824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1808,7 +1835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1819,7 +1846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1830,7 +1857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1841,7 +1868,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1854,8 +1881,11 @@
       <c r="D12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1868,8 +1898,11 @@
       <c r="D13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1883,7 +1916,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1893,8 +1926,11 @@
       <c r="C15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>

</xml_diff>